<commit_message>
change to better examples
</commit_message>
<xml_diff>
--- a/naming_template.xlsx
+++ b/naming_template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Documents\NetBeansProjects\heps-db-naming\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="120" windowWidth="24240" windowHeight="12675" activeTab="3"/>
   </bookViews>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>system_name</t>
   </si>
@@ -37,6 +42,48 @@
   </si>
   <si>
     <t>signal_type</t>
+  </si>
+  <si>
+    <t>LNC</t>
+  </si>
+  <si>
+    <t>Linac</t>
+  </si>
+  <si>
+    <t>BSTR</t>
+  </si>
+  <si>
+    <t>Booster</t>
+  </si>
+  <si>
+    <t>MAG</t>
+  </si>
+  <si>
+    <t>magnet</t>
+  </si>
+  <si>
+    <t>BEND</t>
+  </si>
+  <si>
+    <t>dipole bend</t>
+  </si>
+  <si>
+    <t>QUAD</t>
+  </si>
+  <si>
+    <t>quadrupole</t>
+  </si>
+  <si>
+    <t>Amp_Set</t>
+  </si>
+  <si>
+    <t>amplitude set point</t>
+  </si>
+  <si>
+    <t>I_Set</t>
+  </si>
+  <si>
+    <t>current set point</t>
   </si>
 </sst>
 </file>
@@ -47,13 +94,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -415,7 +462,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -426,12 +473,12 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.375" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -444,19 +491,19 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -470,13 +517,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.125" customWidth="1"/>
-    <col min="2" max="2" width="13.125" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -488,11 +535,11 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>6</v>
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -514,13 +561,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.625" customWidth="1"/>
-    <col min="2" max="2" width="13.625" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -532,19 +579,19 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>12</v>
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -558,12 +605,12 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.125" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -575,19 +622,19 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2">
-        <v>13</v>
-      </c>
-      <c r="B2">
-        <v>14</v>
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3">
-        <v>15</v>
-      </c>
-      <c r="B3">
-        <v>16</v>
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add "comment" field to all tabs in the template.
</commit_message>
<xml_diff>
--- a/naming_template.xlsx
+++ b/naming_template.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul\Documents\NetBeansProjects\heps-db-naming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C.M.P\Documents\NetBeansProjects\heps-db-naming\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{29FD6CFA-43EA-4206-9FE0-9251C41C8FE0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="3" xr2:uid="{10BD2FC0-F91E-47BB-A0BD-8EE16BCD0E5E}"/>
   </bookViews>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>system_name</t>
   </si>
@@ -43,11 +44,14 @@
   <si>
     <t>signal_type</t>
   </si>
+  <si>
+    <t>comment</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -83,8 +87,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{75F42455-B087-4979-A11A-DAC69487EB5F}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -393,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51504206-FD10-43C9-BE38-A7317E69CB58}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,12 +437,15 @@
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -420,10 +455,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8C90A6-2BE2-49FC-BABA-DD72EB2FED3A}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,12 +467,15 @@
     <col min="2" max="2" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -447,10 +485,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E519B1A7-3160-482C-B510-CDA3E0883DE6}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,12 +497,15 @@
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -474,10 +515,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9199315-DF62-46DB-A26D-A9B919DD32BB}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,12 +526,15 @@
     <col min="1" max="1" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>